<commit_message>
updated fuel prices and heat rates
</commit_message>
<xml_diff>
--- a/NG_Bias_Correction/Monthly_fuel_prices/2019_Fuel_Price_Data.xlsx
+++ b/NG_Bias_Correction/Monthly_fuel_prices/2019_Fuel_Price_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkern\Downloads\NG_Bias_Correction\NG_Bias_Correction\Monthly_fuel_prices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkern\Documents\GitHub\IM3_EIC\NG_Bias_Correction\Monthly_fuel_prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="102">
   <si>
     <t>SOCO</t>
   </si>
@@ -307,12 +307,36 @@
   <si>
     <t>NYISO</t>
   </si>
+  <si>
+    <t>NB</t>
+  </si>
+  <si>
+    <t>YAD</t>
+  </si>
+  <si>
+    <t>CPLW</t>
+  </si>
+  <si>
+    <t>SEPA</t>
+  </si>
+  <si>
+    <t>NSB</t>
+  </si>
+  <si>
+    <t>HST</t>
+  </si>
+  <si>
+    <t>EEI</t>
+  </si>
+  <si>
+    <t>GRID</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -325,6 +349,14 @@
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -334,7 +366,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -357,15 +389,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4456,7 +4503,7 @@
   <dimension ref="A1:BB13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -8238,241 +8285,264 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB13"/>
+  <dimension ref="A1:BK13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:63" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="AP1" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="AQ1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="AR1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="BK1" s="2"/>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A2">
+        <v>14.717000000000001</v>
+      </c>
+      <c r="B2">
+        <v>13.5685</v>
+      </c>
+      <c r="C2">
         <v>13.350428571428569</v>
       </c>
-      <c r="B2">
+      <c r="D2">
         <v>13.39522222222222</v>
       </c>
-      <c r="C2">
+      <c r="E2">
         <v>12.64304347826087</v>
       </c>
-      <c r="D2">
+      <c r="F2">
         <v>14.127222222222221</v>
       </c>
-      <c r="E2">
+      <c r="G2">
         <v>14.791</v>
       </c>
-      <c r="F2">
+      <c r="H2">
         <v>13.707470588235299</v>
       </c>
-      <c r="G2">
+      <c r="I2">
         <v>14.16547222222222</v>
       </c>
-      <c r="H2">
+      <c r="J2">
         <v>14.52466666666667</v>
       </c>
-      <c r="I2">
+      <c r="K2">
         <v>14.34733333333333</v>
       </c>
-      <c r="J2">
+      <c r="L2">
         <v>14.157999999999999</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>14.381500000000001</v>
-      </c>
-      <c r="L2">
-        <v>14.52466666666667</v>
-      </c>
-      <c r="M2">
-        <v>16.226216666666669</v>
       </c>
       <c r="N2">
         <v>14.52466666666667</v>
       </c>
       <c r="O2">
-        <v>14.52466666666667</v>
+        <v>16.226216666666669</v>
       </c>
       <c r="P2">
         <v>14.52466666666667</v>
       </c>
       <c r="Q2">
+        <v>14.52466666666667</v>
+      </c>
+      <c r="R2">
+        <v>14.52466666666667</v>
+      </c>
+      <c r="S2">
         <v>19.31733333333333</v>
-      </c>
-      <c r="R2">
-        <v>13.976000000000001</v>
-      </c>
-      <c r="S2">
-        <v>14.79</v>
       </c>
       <c r="T2">
         <v>13.976000000000001</v>
       </c>
       <c r="U2">
-        <v>13.976000000000001</v>
+        <v>14.79</v>
       </c>
       <c r="V2">
         <v>13.976000000000001</v>
@@ -8487,156 +8557,180 @@
         <v>13.976000000000001</v>
       </c>
       <c r="Z2">
+        <v>13.976000000000001</v>
+      </c>
+      <c r="AA2">
+        <v>13.976000000000001</v>
+      </c>
+      <c r="AB2">
+        <v>13.976000000000001</v>
+      </c>
+      <c r="AC2">
+        <v>13.976000000000001</v>
+      </c>
+      <c r="AD2">
         <v>11.406499999999999</v>
       </c>
-      <c r="AA2">
+      <c r="AE2">
         <v>13.400625</v>
       </c>
-      <c r="AB2">
+      <c r="AF2">
         <v>15.638999999999999</v>
       </c>
-      <c r="AC2">
+      <c r="AG2">
+        <v>15.638999999999999</v>
+      </c>
+      <c r="AH2">
         <v>14.211</v>
       </c>
-      <c r="AD2">
+      <c r="AI2">
         <v>14.17</v>
       </c>
-      <c r="AE2">
+      <c r="AJ2">
         <v>19.413499999999999</v>
       </c>
-      <c r="AF2">
+      <c r="AK2">
         <v>24.11</v>
       </c>
-      <c r="AG2">
+      <c r="AL2">
         <v>13.304</v>
       </c>
-      <c r="AH2">
+      <c r="AM2">
         <v>14.438700000000001</v>
       </c>
-      <c r="AI2">
+      <c r="AN2">
         <v>14.321249999999999</v>
       </c>
-      <c r="AJ2">
+      <c r="AO2">
+        <v>14.321249999999999</v>
+      </c>
+      <c r="AP2">
+        <v>14.321249999999999</v>
+      </c>
+      <c r="AQ2">
+        <v>14.321249999999999</v>
+      </c>
+      <c r="AR2">
         <v>14.554</v>
       </c>
-      <c r="AK2">
+      <c r="AS2">
         <v>14.717000000000001</v>
       </c>
-      <c r="AL2">
+      <c r="AT2">
         <v>12.456</v>
-      </c>
-      <c r="AM2">
-        <v>14.79</v>
-      </c>
-      <c r="AN2">
-        <v>13.268599999999999</v>
-      </c>
-      <c r="AO2">
-        <v>14.52466666666667</v>
-      </c>
-      <c r="AP2">
-        <v>14.79</v>
-      </c>
-      <c r="AQ2">
-        <v>14.79</v>
-      </c>
-      <c r="AR2">
-        <v>14.52466666666667</v>
-      </c>
-      <c r="AS2">
-        <v>14.79</v>
-      </c>
-      <c r="AT2">
-        <v>14.52466666666667</v>
       </c>
       <c r="AU2">
         <v>14.79</v>
       </c>
       <c r="AV2">
-        <v>14.79</v>
+        <v>13.268599999999999</v>
       </c>
       <c r="AW2">
-        <v>14.79</v>
+        <v>14.52466666666667</v>
       </c>
       <c r="AX2">
         <v>14.79</v>
       </c>
       <c r="AY2">
-        <v>14.568666666666671</v>
+        <v>14.79</v>
       </c>
       <c r="AZ2">
-        <v>14.79</v>
+        <v>14.52466666666667</v>
       </c>
       <c r="BA2">
         <v>14.79</v>
       </c>
       <c r="BB2">
+        <v>14.52466666666667</v>
+      </c>
+      <c r="BC2">
         <v>14.79</v>
       </c>
+      <c r="BD2">
+        <v>14.79</v>
+      </c>
+      <c r="BE2">
+        <v>14.79</v>
+      </c>
+      <c r="BF2">
+        <v>14.79</v>
+      </c>
+      <c r="BG2">
+        <v>14.568666666666671</v>
+      </c>
+      <c r="BH2">
+        <v>14.79</v>
+      </c>
+      <c r="BI2">
+        <v>14.79</v>
+      </c>
+      <c r="BJ2">
+        <v>14.79</v>
+      </c>
     </row>
-    <row r="3" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A3">
+        <v>20.906500000000001</v>
+      </c>
+      <c r="B3">
+        <v>14.318</v>
+      </c>
+      <c r="C3">
         <v>14.517625000000001</v>
       </c>
-      <c r="B3">
+      <c r="D3">
         <v>14.522</v>
       </c>
-      <c r="C3">
+      <c r="E3">
         <v>15.24702702702703</v>
       </c>
-      <c r="D3">
+      <c r="F3">
         <v>16.394437499999999</v>
       </c>
-      <c r="E3">
+      <c r="G3">
         <v>14.699</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <v>15.235352941176471</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>14.99272222222222</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>14.96666666666667</v>
       </c>
-      <c r="I3">
+      <c r="K3">
         <v>14.82833333333333</v>
       </c>
-      <c r="J3">
+      <c r="L3">
         <v>14.611000000000001</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>15.692500000000001</v>
-      </c>
-      <c r="L3">
-        <v>14.96666666666667</v>
-      </c>
-      <c r="M3">
-        <v>14.864966666666669</v>
       </c>
       <c r="N3">
         <v>14.96666666666667</v>
       </c>
       <c r="O3">
-        <v>14.96666666666667</v>
+        <v>14.864966666666669</v>
       </c>
       <c r="P3">
         <v>14.96666666666667</v>
       </c>
       <c r="Q3">
+        <v>14.96666666666667</v>
+      </c>
+      <c r="R3">
+        <v>14.96666666666667</v>
+      </c>
+      <c r="S3">
         <v>14.67333333333333</v>
-      </c>
-      <c r="R3">
-        <v>15.281000000000001</v>
-      </c>
-      <c r="S3">
-        <v>15.618499999999999</v>
       </c>
       <c r="T3">
         <v>15.281000000000001</v>
       </c>
       <c r="U3">
-        <v>15.281000000000001</v>
+        <v>15.618499999999999</v>
       </c>
       <c r="V3">
         <v>15.281000000000001</v>
@@ -8651,156 +8745,180 @@
         <v>15.281000000000001</v>
       </c>
       <c r="Z3">
+        <v>15.281000000000001</v>
+      </c>
+      <c r="AA3">
+        <v>15.281000000000001</v>
+      </c>
+      <c r="AB3">
+        <v>15.281000000000001</v>
+      </c>
+      <c r="AC3">
+        <v>15.281000000000001</v>
+      </c>
+      <c r="AD3">
         <v>15.5105</v>
       </c>
-      <c r="AA3">
+      <c r="AE3">
         <v>14.58028571428571</v>
       </c>
-      <c r="AB3">
+      <c r="AF3">
         <v>17.335000000000001</v>
       </c>
-      <c r="AC3">
+      <c r="AG3">
+        <v>17.335000000000001</v>
+      </c>
+      <c r="AH3">
         <v>16.242999999999999</v>
       </c>
-      <c r="AD3">
+      <c r="AI3">
         <v>14.69</v>
       </c>
-      <c r="AE3">
+      <c r="AJ3">
         <v>17.643249999999998</v>
       </c>
-      <c r="AF3">
+      <c r="AK3">
         <v>14.38</v>
       </c>
-      <c r="AG3">
+      <c r="AL3">
         <v>13.233000000000001</v>
       </c>
-      <c r="AH3">
+      <c r="AM3">
         <v>14.590999999999999</v>
       </c>
-      <c r="AI3">
+      <c r="AN3">
         <v>14.592000000000001</v>
       </c>
-      <c r="AJ3">
+      <c r="AO3">
+        <v>14.592000000000001</v>
+      </c>
+      <c r="AP3">
+        <v>14.592000000000001</v>
+      </c>
+      <c r="AQ3">
+        <v>14.592000000000001</v>
+      </c>
+      <c r="AR3">
         <v>14.611000000000001</v>
       </c>
-      <c r="AK3">
+      <c r="AS3">
         <v>20.906500000000001</v>
       </c>
-      <c r="AL3">
+      <c r="AT3">
         <v>14.91</v>
-      </c>
-      <c r="AM3">
-        <v>15.618499999999999</v>
-      </c>
-      <c r="AN3">
-        <v>14.964</v>
-      </c>
-      <c r="AO3">
-        <v>14.96666666666667</v>
-      </c>
-      <c r="AP3">
-        <v>15.618499999999999</v>
-      </c>
-      <c r="AQ3">
-        <v>15.618499999999999</v>
-      </c>
-      <c r="AR3">
-        <v>14.96666666666667</v>
-      </c>
-      <c r="AS3">
-        <v>15.618499999999999</v>
-      </c>
-      <c r="AT3">
-        <v>14.96666666666667</v>
       </c>
       <c r="AU3">
         <v>15.618499999999999</v>
       </c>
       <c r="AV3">
-        <v>15.618499999999999</v>
+        <v>14.964</v>
       </c>
       <c r="AW3">
-        <v>15.618499999999999</v>
+        <v>14.96666666666667</v>
       </c>
       <c r="AX3">
         <v>15.618499999999999</v>
       </c>
       <c r="AY3">
-        <v>15.223416666666671</v>
+        <v>15.618499999999999</v>
       </c>
       <c r="AZ3">
-        <v>15.618499999999999</v>
+        <v>14.96666666666667</v>
       </c>
       <c r="BA3">
         <v>15.618499999999999</v>
       </c>
       <c r="BB3">
+        <v>14.96666666666667</v>
+      </c>
+      <c r="BC3">
         <v>15.618499999999999</v>
       </c>
+      <c r="BD3">
+        <v>15.618499999999999</v>
+      </c>
+      <c r="BE3">
+        <v>15.618499999999999</v>
+      </c>
+      <c r="BF3">
+        <v>15.618499999999999</v>
+      </c>
+      <c r="BG3">
+        <v>15.223416666666671</v>
+      </c>
+      <c r="BH3">
+        <v>15.618499999999999</v>
+      </c>
+      <c r="BI3">
+        <v>15.618499999999999</v>
+      </c>
+      <c r="BJ3">
+        <v>15.618499999999999</v>
+      </c>
     </row>
-    <row r="4" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A4">
+        <v>14.4072</v>
+      </c>
+      <c r="B4">
+        <v>14.799799999999999</v>
+      </c>
+      <c r="C4">
         <v>14.567666666666669</v>
       </c>
-      <c r="B4">
+      <c r="D4">
         <v>14.995875</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>15.08378260869565</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>16.276473684210529</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>15.696</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>15.12721428571429</v>
       </c>
-      <c r="G4">
+      <c r="I4">
         <v>17.53766666666667</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>15.497999999999999</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>15.194000000000001</v>
       </c>
-      <c r="J4">
+      <c r="L4">
         <v>16.3065</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>16.017499999999998</v>
-      </c>
-      <c r="L4">
-        <v>15.497999999999999</v>
-      </c>
-      <c r="M4">
-        <v>16.694199999999999</v>
       </c>
       <c r="N4">
         <v>15.497999999999999</v>
       </c>
       <c r="O4">
-        <v>15.497999999999999</v>
+        <v>16.694199999999999</v>
       </c>
       <c r="P4">
         <v>15.497999999999999</v>
       </c>
       <c r="Q4">
+        <v>15.497999999999999</v>
+      </c>
+      <c r="R4">
+        <v>15.497999999999999</v>
+      </c>
+      <c r="S4">
         <v>15.429</v>
-      </c>
-      <c r="R4">
-        <v>16.077999999999999</v>
-      </c>
-      <c r="S4">
-        <v>21.523</v>
       </c>
       <c r="T4">
         <v>16.077999999999999</v>
       </c>
       <c r="U4">
-        <v>16.077999999999999</v>
+        <v>21.523</v>
       </c>
       <c r="V4">
         <v>16.077999999999999</v>
@@ -8815,156 +8933,180 @@
         <v>16.077999999999999</v>
       </c>
       <c r="Z4">
+        <v>16.077999999999999</v>
+      </c>
+      <c r="AA4">
+        <v>16.077999999999999</v>
+      </c>
+      <c r="AB4">
+        <v>16.077999999999999</v>
+      </c>
+      <c r="AC4">
+        <v>16.077999999999999</v>
+      </c>
+      <c r="AD4">
         <v>15.815</v>
       </c>
-      <c r="AA4">
+      <c r="AE4">
         <v>15.042444444444451</v>
       </c>
-      <c r="AB4">
+      <c r="AF4">
         <v>17.672333333333331</v>
       </c>
-      <c r="AC4">
+      <c r="AG4">
+        <v>17.672333333333331</v>
+      </c>
+      <c r="AH4">
         <v>16.908000000000001</v>
       </c>
-      <c r="AD4">
+      <c r="AI4">
         <v>14.89</v>
       </c>
-      <c r="AE4">
+      <c r="AJ4">
         <v>14.883599999999999</v>
       </c>
-      <c r="AF4">
+      <c r="AK4">
         <v>15.36</v>
       </c>
-      <c r="AG4">
+      <c r="AL4">
         <v>15.891</v>
       </c>
-      <c r="AH4">
+      <c r="AM4">
         <v>15.928750000000001</v>
       </c>
-      <c r="AI4">
+      <c r="AN4">
         <v>15.551</v>
       </c>
-      <c r="AJ4">
+      <c r="AO4">
+        <v>15.551</v>
+      </c>
+      <c r="AP4">
+        <v>15.551</v>
+      </c>
+      <c r="AQ4">
+        <v>15.551</v>
+      </c>
+      <c r="AR4">
         <v>16.3065</v>
       </c>
-      <c r="AK4">
+      <c r="AS4">
         <v>15.032</v>
       </c>
-      <c r="AL4">
+      <c r="AT4">
         <v>19.545999999999999</v>
-      </c>
-      <c r="AM4">
-        <v>21.523</v>
-      </c>
-      <c r="AN4">
-        <v>15.4702</v>
-      </c>
-      <c r="AO4">
-        <v>15.497999999999999</v>
-      </c>
-      <c r="AP4">
-        <v>21.523</v>
-      </c>
-      <c r="AQ4">
-        <v>21.523</v>
-      </c>
-      <c r="AR4">
-        <v>15.497999999999999</v>
-      </c>
-      <c r="AS4">
-        <v>21.523</v>
-      </c>
-      <c r="AT4">
-        <v>15.497999999999999</v>
       </c>
       <c r="AU4">
         <v>21.523</v>
       </c>
       <c r="AV4">
-        <v>21.523</v>
+        <v>15.4702</v>
       </c>
       <c r="AW4">
-        <v>21.523</v>
+        <v>15.497999999999999</v>
       </c>
       <c r="AX4">
         <v>21.523</v>
       </c>
       <c r="AY4">
-        <v>18.358499999999999</v>
+        <v>21.523</v>
       </c>
       <c r="AZ4">
-        <v>21.523</v>
+        <v>15.497999999999999</v>
       </c>
       <c r="BA4">
         <v>21.523</v>
       </c>
       <c r="BB4">
+        <v>15.497999999999999</v>
+      </c>
+      <c r="BC4">
         <v>21.523</v>
       </c>
+      <c r="BD4">
+        <v>21.523</v>
+      </c>
+      <c r="BE4">
+        <v>21.523</v>
+      </c>
+      <c r="BF4">
+        <v>21.523</v>
+      </c>
+      <c r="BG4">
+        <v>18.358499999999999</v>
+      </c>
+      <c r="BH4">
+        <v>21.523</v>
+      </c>
+      <c r="BI4">
+        <v>21.523</v>
+      </c>
+      <c r="BJ4">
+        <v>21.523</v>
+      </c>
     </row>
-    <row r="5" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A5">
+        <v>14.689399999999999</v>
+      </c>
+      <c r="B5">
+        <v>15.6196</v>
+      </c>
+      <c r="C5">
         <v>14.9076</v>
       </c>
-      <c r="B5">
+      <c r="D5">
         <v>15.591142857142859</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>15.373794871794869</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>16.128055555555559</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>16.035</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>15.646294117647059</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>17.536888888888889</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>17.56066666666667</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>16.66033333333333</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <v>15.741</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>16.361000000000001</v>
-      </c>
-      <c r="L5">
-        <v>17.56066666666667</v>
-      </c>
-      <c r="M5">
-        <v>17.966266666666659</v>
       </c>
       <c r="N5">
         <v>17.56066666666667</v>
       </c>
       <c r="O5">
-        <v>17.56066666666667</v>
+        <v>17.966266666666659</v>
       </c>
       <c r="P5">
         <v>17.56066666666667</v>
       </c>
       <c r="Q5">
+        <v>17.56066666666667</v>
+      </c>
+      <c r="R5">
+        <v>17.56066666666667</v>
+      </c>
+      <c r="S5">
         <v>18.61033333333333</v>
-      </c>
-      <c r="R5">
-        <v>16.306999999999999</v>
-      </c>
-      <c r="S5">
-        <v>17.9405</v>
       </c>
       <c r="T5">
         <v>16.306999999999999</v>
       </c>
       <c r="U5">
-        <v>16.306999999999999</v>
+        <v>17.9405</v>
       </c>
       <c r="V5">
         <v>16.306999999999999</v>
@@ -8979,156 +9121,180 @@
         <v>16.306999999999999</v>
       </c>
       <c r="Z5">
+        <v>16.306999999999999</v>
+      </c>
+      <c r="AA5">
+        <v>16.306999999999999</v>
+      </c>
+      <c r="AB5">
+        <v>16.306999999999999</v>
+      </c>
+      <c r="AC5">
+        <v>16.306999999999999</v>
+      </c>
+      <c r="AD5">
         <v>16.0185</v>
       </c>
-      <c r="AA5">
+      <c r="AE5">
         <v>15.232714285714289</v>
       </c>
-      <c r="AB5">
+      <c r="AF5">
         <v>17.952000000000002</v>
       </c>
-      <c r="AC5">
+      <c r="AG5">
+        <v>17.952000000000002</v>
+      </c>
+      <c r="AH5">
         <v>16.829999999999998</v>
       </c>
-      <c r="AD5">
+      <c r="AI5">
         <v>15.76</v>
       </c>
-      <c r="AE5">
+      <c r="AJ5">
         <v>17.174700000000001</v>
       </c>
-      <c r="AF5">
+      <c r="AK5">
         <v>19.66</v>
       </c>
-      <c r="AG5">
+      <c r="AL5">
         <v>20.49</v>
       </c>
-      <c r="AH5">
+      <c r="AM5">
         <v>15.868499999999999</v>
       </c>
-      <c r="AI5">
+      <c r="AN5">
         <v>15.64575</v>
       </c>
-      <c r="AJ5">
+      <c r="AO5">
+        <v>15.64575</v>
+      </c>
+      <c r="AP5">
+        <v>15.64575</v>
+      </c>
+      <c r="AQ5">
+        <v>15.64575</v>
+      </c>
+      <c r="AR5">
         <v>16.091249999999999</v>
       </c>
-      <c r="AK5">
+      <c r="AS5">
         <v>15.227333333333331</v>
       </c>
-      <c r="AL5">
+      <c r="AT5">
         <v>17.524999999999999</v>
-      </c>
-      <c r="AM5">
-        <v>17.9405</v>
-      </c>
-      <c r="AN5">
-        <v>15.749124999999999</v>
-      </c>
-      <c r="AO5">
-        <v>17.56066666666667</v>
-      </c>
-      <c r="AP5">
-        <v>17.9405</v>
-      </c>
-      <c r="AQ5">
-        <v>17.9405</v>
-      </c>
-      <c r="AR5">
-        <v>17.56066666666667</v>
-      </c>
-      <c r="AS5">
-        <v>17.9405</v>
-      </c>
-      <c r="AT5">
-        <v>17.56066666666667</v>
       </c>
       <c r="AU5">
         <v>17.9405</v>
       </c>
       <c r="AV5">
-        <v>17.9405</v>
+        <v>15.749124999999999</v>
       </c>
       <c r="AW5">
-        <v>17.9405</v>
+        <v>17.56066666666667</v>
       </c>
       <c r="AX5">
         <v>17.9405</v>
       </c>
       <c r="AY5">
-        <v>17.300416666666671</v>
+        <v>17.9405</v>
       </c>
       <c r="AZ5">
-        <v>17.9405</v>
+        <v>17.56066666666667</v>
       </c>
       <c r="BA5">
         <v>17.9405</v>
       </c>
       <c r="BB5">
+        <v>17.56066666666667</v>
+      </c>
+      <c r="BC5">
         <v>17.9405</v>
       </c>
+      <c r="BD5">
+        <v>17.9405</v>
+      </c>
+      <c r="BE5">
+        <v>17.9405</v>
+      </c>
+      <c r="BF5">
+        <v>17.9405</v>
+      </c>
+      <c r="BG5">
+        <v>17.300416666666671</v>
+      </c>
+      <c r="BH5">
+        <v>17.9405</v>
+      </c>
+      <c r="BI5">
+        <v>17.9405</v>
+      </c>
+      <c r="BJ5">
+        <v>17.9405</v>
+      </c>
     </row>
-    <row r="6" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A6">
+        <v>15.3652</v>
+      </c>
+      <c r="B6">
+        <v>15.256666666666669</v>
+      </c>
+      <c r="C6">
         <v>15.98</v>
       </c>
-      <c r="B6">
+      <c r="D6">
         <v>15.41977777777778</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>15.61409756097561</v>
       </c>
-      <c r="D6">
+      <c r="F6">
         <v>16.284062500000001</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <v>15.907999999999999</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>15.644722222222221</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>18.052472222222221</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>17.932749999999999</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>17.116375000000001</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <v>15.637</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <v>16.41</v>
-      </c>
-      <c r="L6">
-        <v>17.932749999999999</v>
-      </c>
-      <c r="M6">
-        <v>17.990033333333329</v>
       </c>
       <c r="N6">
         <v>17.932749999999999</v>
       </c>
       <c r="O6">
-        <v>17.932749999999999</v>
+        <v>17.990033333333329</v>
       </c>
       <c r="P6">
         <v>17.932749999999999</v>
       </c>
       <c r="Q6">
+        <v>17.932749999999999</v>
+      </c>
+      <c r="R6">
+        <v>17.932749999999999</v>
+      </c>
+      <c r="S6">
         <v>17.896374999999999</v>
-      </c>
-      <c r="R6">
-        <v>16.130749999999999</v>
-      </c>
-      <c r="S6">
-        <v>18.269666666666669</v>
       </c>
       <c r="T6">
         <v>16.130749999999999</v>
       </c>
       <c r="U6">
-        <v>16.130749999999999</v>
+        <v>18.269666666666669</v>
       </c>
       <c r="V6">
         <v>16.130749999999999</v>
@@ -9143,156 +9309,180 @@
         <v>16.130749999999999</v>
       </c>
       <c r="Z6">
+        <v>16.130749999999999</v>
+      </c>
+      <c r="AA6">
+        <v>16.130749999999999</v>
+      </c>
+      <c r="AB6">
+        <v>16.130749999999999</v>
+      </c>
+      <c r="AC6">
+        <v>16.130749999999999</v>
+      </c>
+      <c r="AD6">
         <v>16.181000000000001</v>
       </c>
-      <c r="AA6">
+      <c r="AE6">
         <v>15.348444444444439</v>
       </c>
-      <c r="AB6">
+      <c r="AF6">
         <v>18.951000000000001</v>
       </c>
-      <c r="AC6">
+      <c r="AG6">
+        <v>18.951000000000001</v>
+      </c>
+      <c r="AH6">
         <v>16.232500000000002</v>
       </c>
-      <c r="AD6">
+      <c r="AI6">
         <v>16.3</v>
       </c>
-      <c r="AE6">
+      <c r="AJ6">
         <v>16.6126</v>
       </c>
-      <c r="AF6">
+      <c r="AK6">
         <v>17.86</v>
       </c>
-      <c r="AG6">
+      <c r="AL6">
         <v>18.292999999999999</v>
       </c>
-      <c r="AH6">
+      <c r="AM6">
         <v>15.50783333333333</v>
       </c>
-      <c r="AI6">
+      <c r="AN6">
         <v>15.4695</v>
       </c>
-      <c r="AJ6">
+      <c r="AO6">
+        <v>15.4695</v>
+      </c>
+      <c r="AP6">
+        <v>15.4695</v>
+      </c>
+      <c r="AQ6">
+        <v>15.4695</v>
+      </c>
+      <c r="AR6">
         <v>15.718666666666669</v>
       </c>
-      <c r="AK6">
+      <c r="AS6">
         <v>16.009</v>
       </c>
-      <c r="AL6">
+      <c r="AT6">
         <v>18.350249999999999</v>
-      </c>
-      <c r="AM6">
-        <v>18.269666666666669</v>
-      </c>
-      <c r="AN6">
-        <v>15.72290909090909</v>
-      </c>
-      <c r="AO6">
-        <v>17.932749999999999</v>
-      </c>
-      <c r="AP6">
-        <v>18.269666666666669</v>
-      </c>
-      <c r="AQ6">
-        <v>18.269666666666669</v>
-      </c>
-      <c r="AR6">
-        <v>17.932749999999999</v>
-      </c>
-      <c r="AS6">
-        <v>18.269666666666669</v>
-      </c>
-      <c r="AT6">
-        <v>17.932749999999999</v>
       </c>
       <c r="AU6">
         <v>18.269666666666669</v>
       </c>
       <c r="AV6">
-        <v>18.269666666666669</v>
+        <v>15.72290909090909</v>
       </c>
       <c r="AW6">
-        <v>18.269666666666669</v>
+        <v>17.932749999999999</v>
       </c>
       <c r="AX6">
         <v>18.269666666666669</v>
       </c>
       <c r="AY6">
-        <v>17.693020833333328</v>
+        <v>18.269666666666669</v>
       </c>
       <c r="AZ6">
-        <v>18.269666666666669</v>
+        <v>17.932749999999999</v>
       </c>
       <c r="BA6">
         <v>18.269666666666669</v>
       </c>
       <c r="BB6">
+        <v>17.932749999999999</v>
+      </c>
+      <c r="BC6">
         <v>18.269666666666669</v>
       </c>
+      <c r="BD6">
+        <v>18.269666666666669</v>
+      </c>
+      <c r="BE6">
+        <v>18.269666666666669</v>
+      </c>
+      <c r="BF6">
+        <v>18.269666666666669</v>
+      </c>
+      <c r="BG6">
+        <v>17.693020833333328</v>
+      </c>
+      <c r="BH6">
+        <v>18.269666666666669</v>
+      </c>
+      <c r="BI6">
+        <v>18.269666666666669</v>
+      </c>
+      <c r="BJ6">
+        <v>18.269666666666669</v>
+      </c>
     </row>
-    <row r="7" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>15.278</v>
+        <v>14.560750000000001</v>
       </c>
       <c r="B7">
         <v>13.970499999999999</v>
       </c>
       <c r="C7">
+        <v>15.278</v>
+      </c>
+      <c r="D7">
+        <v>13.970499999999999</v>
+      </c>
+      <c r="E7">
         <v>13.612363636363639</v>
       </c>
-      <c r="D7">
+      <c r="F7">
         <v>15.170352941176469</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <v>14.563000000000001</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>13.9959375</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>15.496833333333329</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>17.25525</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>17.047625</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <v>14.8125</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>14.9695</v>
-      </c>
-      <c r="L7">
-        <v>17.25525</v>
-      </c>
-      <c r="M7">
-        <v>16.587150000000001</v>
       </c>
       <c r="N7">
         <v>17.25525</v>
       </c>
       <c r="O7">
-        <v>17.25525</v>
+        <v>16.587150000000001</v>
       </c>
       <c r="P7">
         <v>17.25525</v>
       </c>
       <c r="Q7">
+        <v>17.25525</v>
+      </c>
+      <c r="R7">
+        <v>17.25525</v>
+      </c>
+      <c r="S7">
         <v>18.222625000000001</v>
-      </c>
-      <c r="R7">
-        <v>14.816333333333329</v>
-      </c>
-      <c r="S7">
-        <v>14.08075</v>
       </c>
       <c r="T7">
         <v>14.816333333333329</v>
       </c>
       <c r="U7">
-        <v>14.816333333333329</v>
+        <v>14.08075</v>
       </c>
       <c r="V7">
         <v>14.816333333333329</v>
@@ -9307,156 +9497,180 @@
         <v>14.816333333333329</v>
       </c>
       <c r="Z7">
+        <v>14.816333333333329</v>
+      </c>
+      <c r="AA7">
+        <v>14.816333333333329</v>
+      </c>
+      <c r="AB7">
+        <v>14.816333333333329</v>
+      </c>
+      <c r="AC7">
+        <v>14.816333333333329</v>
+      </c>
+      <c r="AD7">
         <v>14.452</v>
       </c>
-      <c r="AA7">
+      <c r="AE7">
         <v>13.891</v>
       </c>
-      <c r="AB7">
+      <c r="AF7">
         <v>16.913</v>
       </c>
-      <c r="AC7">
+      <c r="AG7">
+        <v>16.913</v>
+      </c>
+      <c r="AH7">
         <v>14.952</v>
       </c>
-      <c r="AD7">
+      <c r="AI7">
         <v>16.84</v>
       </c>
-      <c r="AE7">
+      <c r="AJ7">
         <v>16.875374999999998</v>
       </c>
-      <c r="AF7">
+      <c r="AK7">
         <v>19.190000000000001</v>
       </c>
-      <c r="AG7">
+      <c r="AL7">
         <v>14.15</v>
       </c>
-      <c r="AH7">
+      <c r="AM7">
         <v>14.495708333333329</v>
       </c>
-      <c r="AI7">
+      <c r="AN7">
         <v>13.992749999999999</v>
       </c>
-      <c r="AJ7">
+      <c r="AO7">
+        <v>13.992749999999999</v>
+      </c>
+      <c r="AP7">
+        <v>13.992749999999999</v>
+      </c>
+      <c r="AQ7">
+        <v>13.992749999999999</v>
+      </c>
+      <c r="AR7">
         <v>14.99866666666667</v>
       </c>
-      <c r="AK7">
+      <c r="AS7">
         <v>14.727</v>
       </c>
-      <c r="AL7">
+      <c r="AT7">
         <v>14.198499999999999</v>
-      </c>
-      <c r="AM7">
-        <v>14.08075</v>
-      </c>
-      <c r="AN7">
-        <v>14.152714285714289</v>
-      </c>
-      <c r="AO7">
-        <v>17.25525</v>
-      </c>
-      <c r="AP7">
-        <v>14.08075</v>
-      </c>
-      <c r="AQ7">
-        <v>14.08075</v>
-      </c>
-      <c r="AR7">
-        <v>17.25525</v>
-      </c>
-      <c r="AS7">
-        <v>14.08075</v>
-      </c>
-      <c r="AT7">
-        <v>17.25525</v>
       </c>
       <c r="AU7">
         <v>14.08075</v>
       </c>
       <c r="AV7">
-        <v>14.08075</v>
+        <v>14.152714285714289</v>
       </c>
       <c r="AW7">
-        <v>14.08075</v>
+        <v>17.25525</v>
       </c>
       <c r="AX7">
         <v>14.08075</v>
       </c>
       <c r="AY7">
-        <v>15.564187499999999</v>
+        <v>14.08075</v>
       </c>
       <c r="AZ7">
-        <v>14.08075</v>
+        <v>17.25525</v>
       </c>
       <c r="BA7">
         <v>14.08075</v>
       </c>
       <c r="BB7">
+        <v>17.25525</v>
+      </c>
+      <c r="BC7">
         <v>14.08075</v>
       </c>
+      <c r="BD7">
+        <v>14.08075</v>
+      </c>
+      <c r="BE7">
+        <v>14.08075</v>
+      </c>
+      <c r="BF7">
+        <v>14.08075</v>
+      </c>
+      <c r="BG7">
+        <v>15.564187499999999</v>
+      </c>
+      <c r="BH7">
+        <v>14.08075</v>
+      </c>
+      <c r="BI7">
+        <v>14.08075</v>
+      </c>
+      <c r="BJ7">
+        <v>14.08075</v>
+      </c>
     </row>
-    <row r="8" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A8">
+        <v>15.15225</v>
+      </c>
+      <c r="B8">
+        <v>13.993124999999999</v>
+      </c>
+      <c r="C8">
         <v>14.78914285714286</v>
       </c>
-      <c r="B8">
+      <c r="D8">
         <v>14.138727272727269</v>
       </c>
-      <c r="C8">
+      <c r="E8">
         <v>15.17864102564103</v>
       </c>
-      <c r="D8">
+      <c r="F8">
         <v>15.43170588235294</v>
       </c>
-      <c r="E8">
+      <c r="G8">
         <v>15.217000000000001</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>14.723571428571431</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>15.184111111111109</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>16.259499999999999</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>16.84975</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <v>14.696999999999999</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <v>15.523</v>
-      </c>
-      <c r="L8">
-        <v>16.259499999999999</v>
-      </c>
-      <c r="M8">
-        <v>16.218366666666672</v>
       </c>
       <c r="N8">
         <v>16.259499999999999</v>
       </c>
       <c r="O8">
-        <v>16.259499999999999</v>
+        <v>16.218366666666672</v>
       </c>
       <c r="P8">
         <v>16.259499999999999</v>
       </c>
       <c r="Q8">
+        <v>16.259499999999999</v>
+      </c>
+      <c r="R8">
+        <v>16.259499999999999</v>
+      </c>
+      <c r="S8">
         <v>17.769749999999998</v>
-      </c>
-      <c r="R8">
-        <v>15.203250000000001</v>
-      </c>
-      <c r="S8">
-        <v>15.044333333333331</v>
       </c>
       <c r="T8">
         <v>15.203250000000001</v>
       </c>
       <c r="U8">
-        <v>15.203250000000001</v>
+        <v>15.044333333333331</v>
       </c>
       <c r="V8">
         <v>15.203250000000001</v>
@@ -9471,156 +9685,180 @@
         <v>15.203250000000001</v>
       </c>
       <c r="Z8">
+        <v>15.203250000000001</v>
+      </c>
+      <c r="AA8">
+        <v>15.203250000000001</v>
+      </c>
+      <c r="AB8">
+        <v>15.203250000000001</v>
+      </c>
+      <c r="AC8">
+        <v>15.203250000000001</v>
+      </c>
+      <c r="AD8">
         <v>14.641</v>
       </c>
-      <c r="AA8">
+      <c r="AE8">
         <v>14.19014285714286</v>
       </c>
-      <c r="AB8">
+      <c r="AF8">
         <v>17.972999999999999</v>
       </c>
-      <c r="AC8">
+      <c r="AG8">
+        <v>17.972999999999999</v>
+      </c>
+      <c r="AH8">
         <v>15.92</v>
       </c>
-      <c r="AD8">
+      <c r="AI8">
         <v>17.440000000000001</v>
       </c>
-      <c r="AE8">
+      <c r="AJ8">
         <v>17.216125000000002</v>
       </c>
-      <c r="AF8">
+      <c r="AK8">
         <v>19.28</v>
       </c>
-      <c r="AG8">
+      <c r="AL8">
         <v>16.669</v>
       </c>
-      <c r="AH8">
+      <c r="AM8">
         <v>14.703250000000001</v>
       </c>
-      <c r="AI8">
+      <c r="AN8">
         <v>14.5665</v>
       </c>
-      <c r="AJ8">
+      <c r="AO8">
+        <v>14.5665</v>
+      </c>
+      <c r="AP8">
+        <v>14.5665</v>
+      </c>
+      <c r="AQ8">
+        <v>14.5665</v>
+      </c>
+      <c r="AR8">
         <v>14.84</v>
       </c>
-      <c r="AK8">
+      <c r="AS8">
         <v>15.34433333333333</v>
       </c>
-      <c r="AL8">
+      <c r="AT8">
         <v>14.67975</v>
-      </c>
-      <c r="AM8">
-        <v>15.044333333333331</v>
-      </c>
-      <c r="AN8">
-        <v>14.6656</v>
-      </c>
-      <c r="AO8">
-        <v>16.259499999999999</v>
-      </c>
-      <c r="AP8">
-        <v>15.044333333333331</v>
-      </c>
-      <c r="AQ8">
-        <v>15.044333333333331</v>
-      </c>
-      <c r="AR8">
-        <v>16.259499999999999</v>
-      </c>
-      <c r="AS8">
-        <v>15.044333333333331</v>
-      </c>
-      <c r="AT8">
-        <v>16.259499999999999</v>
       </c>
       <c r="AU8">
         <v>15.044333333333331</v>
       </c>
       <c r="AV8">
-        <v>15.044333333333331</v>
+        <v>14.6656</v>
       </c>
       <c r="AW8">
-        <v>15.044333333333331</v>
+        <v>16.259499999999999</v>
       </c>
       <c r="AX8">
         <v>15.044333333333331</v>
       </c>
       <c r="AY8">
-        <v>15.947041666666671</v>
+        <v>15.044333333333331</v>
       </c>
       <c r="AZ8">
-        <v>15.044333333333331</v>
+        <v>16.259499999999999</v>
       </c>
       <c r="BA8">
         <v>15.044333333333331</v>
       </c>
       <c r="BB8">
+        <v>16.259499999999999</v>
+      </c>
+      <c r="BC8">
         <v>15.044333333333331</v>
       </c>
+      <c r="BD8">
+        <v>15.044333333333331</v>
+      </c>
+      <c r="BE8">
+        <v>15.044333333333331</v>
+      </c>
+      <c r="BF8">
+        <v>15.044333333333331</v>
+      </c>
+      <c r="BG8">
+        <v>15.947041666666671</v>
+      </c>
+      <c r="BH8">
+        <v>15.044333333333331</v>
+      </c>
+      <c r="BI8">
+        <v>15.044333333333331</v>
+      </c>
+      <c r="BJ8">
+        <v>15.044333333333331</v>
+      </c>
     </row>
-    <row r="9" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A9">
+        <v>14.72275</v>
+      </c>
+      <c r="B9">
+        <v>13.545999999999999</v>
+      </c>
+      <c r="C9">
         <v>14.215285714285709</v>
       </c>
-      <c r="B9">
+      <c r="D9">
         <v>13.77911111111111</v>
       </c>
-      <c r="C9">
+      <c r="E9">
         <v>13.77331818181818</v>
       </c>
-      <c r="D9">
+      <c r="F9">
         <v>15.180055555555549</v>
       </c>
-      <c r="E9">
+      <c r="G9">
         <v>14.617000000000001</v>
       </c>
-      <c r="F9">
+      <c r="H9">
         <v>14.084199999999999</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>15.95586111111111</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>16.84033333333333</v>
       </c>
-      <c r="I9">
+      <c r="K9">
         <v>17.075166666666671</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <v>14.145</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <v>14.891</v>
-      </c>
-      <c r="L9">
-        <v>16.84033333333333</v>
-      </c>
-      <c r="M9">
-        <v>17.00558333333333</v>
       </c>
       <c r="N9">
         <v>16.84033333333333</v>
       </c>
       <c r="O9">
-        <v>16.84033333333333</v>
+        <v>17.00558333333333</v>
       </c>
       <c r="P9">
         <v>16.84033333333333</v>
       </c>
       <c r="Q9">
+        <v>16.84033333333333</v>
+      </c>
+      <c r="R9">
+        <v>16.84033333333333</v>
+      </c>
+      <c r="S9">
         <v>18.58016666666667</v>
-      </c>
-      <c r="R9">
-        <v>14.171714285714289</v>
-      </c>
-      <c r="S9">
-        <v>15.00825</v>
       </c>
       <c r="T9">
         <v>14.171714285714289</v>
       </c>
       <c r="U9">
-        <v>14.171714285714289</v>
+        <v>15.00825</v>
       </c>
       <c r="V9">
         <v>14.171714285714289</v>
@@ -9635,156 +9873,180 @@
         <v>14.171714285714289</v>
       </c>
       <c r="Z9">
+        <v>14.171714285714289</v>
+      </c>
+      <c r="AA9">
+        <v>14.171714285714289</v>
+      </c>
+      <c r="AB9">
+        <v>14.171714285714289</v>
+      </c>
+      <c r="AC9">
+        <v>14.171714285714289</v>
+      </c>
+      <c r="AD9">
         <v>14.432499999999999</v>
       </c>
-      <c r="AA9">
+      <c r="AE9">
         <v>13.95485714285714</v>
       </c>
-      <c r="AB9">
+      <c r="AF9">
         <v>18.630500000000001</v>
       </c>
-      <c r="AC9">
+      <c r="AG9">
+        <v>18.630500000000001</v>
+      </c>
+      <c r="AH9">
         <v>15.446999999999999</v>
       </c>
-      <c r="AD9">
+      <c r="AI9">
         <v>17.309999999999999</v>
       </c>
-      <c r="AE9">
+      <c r="AJ9">
         <v>17.521374999999999</v>
       </c>
-      <c r="AF9">
+      <c r="AK9">
         <v>20.32</v>
       </c>
-      <c r="AG9">
+      <c r="AL9">
         <v>18.715</v>
       </c>
-      <c r="AH9">
+      <c r="AM9">
         <v>14.136791666666671</v>
       </c>
-      <c r="AI9">
+      <c r="AN9">
         <v>13.943250000000001</v>
       </c>
-      <c r="AJ9">
+      <c r="AO9">
+        <v>13.943250000000001</v>
+      </c>
+      <c r="AP9">
+        <v>13.943250000000001</v>
+      </c>
+      <c r="AQ9">
+        <v>13.943250000000001</v>
+      </c>
+      <c r="AR9">
         <v>14.33033333333333</v>
       </c>
-      <c r="AK9">
+      <c r="AS9">
         <v>14.824999999999999</v>
       </c>
-      <c r="AL9">
+      <c r="AT9">
         <v>15.39</v>
-      </c>
-      <c r="AM9">
-        <v>15.00825</v>
-      </c>
-      <c r="AN9">
-        <v>14.0709</v>
-      </c>
-      <c r="AO9">
-        <v>16.84033333333333</v>
-      </c>
-      <c r="AP9">
-        <v>15.00825</v>
-      </c>
-      <c r="AQ9">
-        <v>15.00825</v>
-      </c>
-      <c r="AR9">
-        <v>16.84033333333333</v>
-      </c>
-      <c r="AS9">
-        <v>15.00825</v>
-      </c>
-      <c r="AT9">
-        <v>16.84033333333333</v>
       </c>
       <c r="AU9">
         <v>15.00825</v>
       </c>
       <c r="AV9">
-        <v>15.00825</v>
+        <v>14.0709</v>
       </c>
       <c r="AW9">
-        <v>15.00825</v>
+        <v>16.84033333333333</v>
       </c>
       <c r="AX9">
         <v>15.00825</v>
       </c>
       <c r="AY9">
-        <v>16.041708333333329</v>
+        <v>15.00825</v>
       </c>
       <c r="AZ9">
-        <v>15.00825</v>
+        <v>16.84033333333333</v>
       </c>
       <c r="BA9">
         <v>15.00825</v>
       </c>
       <c r="BB9">
+        <v>16.84033333333333</v>
+      </c>
+      <c r="BC9">
         <v>15.00825</v>
       </c>
+      <c r="BD9">
+        <v>15.00825</v>
+      </c>
+      <c r="BE9">
+        <v>15.00825</v>
+      </c>
+      <c r="BF9">
+        <v>15.00825</v>
+      </c>
+      <c r="BG9">
+        <v>16.041708333333329</v>
+      </c>
+      <c r="BH9">
+        <v>15.00825</v>
+      </c>
+      <c r="BI9">
+        <v>15.00825</v>
+      </c>
+      <c r="BJ9">
+        <v>15.00825</v>
+      </c>
     </row>
-    <row r="10" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A10">
+        <v>14.952</v>
+      </c>
+      <c r="B10">
+        <v>14.50542857142857</v>
+      </c>
+      <c r="C10">
         <v>14.795999999999999</v>
       </c>
-      <c r="B10">
+      <c r="D10">
         <v>14.686299999999999</v>
       </c>
-      <c r="C10">
+      <c r="E10">
         <v>14.043525000000001</v>
       </c>
-      <c r="D10">
+      <c r="F10">
         <v>13.63927777777778</v>
       </c>
-      <c r="E10">
+      <c r="G10">
         <v>15.417</v>
       </c>
-      <c r="F10">
+      <c r="H10">
         <v>14.67911764705882</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>15.96544444444444</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>14.327</v>
       </c>
-      <c r="I10">
+      <c r="K10">
         <v>15.4735</v>
       </c>
-      <c r="J10">
+      <c r="L10">
         <v>14.794499999999999</v>
       </c>
-      <c r="K10">
+      <c r="M10">
         <v>15.862500000000001</v>
-      </c>
-      <c r="L10">
-        <v>14.327</v>
-      </c>
-      <c r="M10">
-        <v>16.266666666666669</v>
       </c>
       <c r="N10">
         <v>14.327</v>
       </c>
       <c r="O10">
-        <v>14.327</v>
+        <v>16.266666666666669</v>
       </c>
       <c r="P10">
         <v>14.327</v>
       </c>
       <c r="Q10">
+        <v>14.327</v>
+      </c>
+      <c r="R10">
+        <v>14.327</v>
+      </c>
+      <c r="S10">
         <v>16.718499999999999</v>
-      </c>
-      <c r="R10">
-        <v>15.5075</v>
-      </c>
-      <c r="S10">
-        <v>16.572333333333329</v>
       </c>
       <c r="T10">
         <v>15.5075</v>
       </c>
       <c r="U10">
-        <v>15.5075</v>
+        <v>16.572333333333329</v>
       </c>
       <c r="V10">
         <v>15.5075</v>
@@ -9799,156 +10061,180 @@
         <v>15.5075</v>
       </c>
       <c r="Z10">
+        <v>15.5075</v>
+      </c>
+      <c r="AA10">
+        <v>15.5075</v>
+      </c>
+      <c r="AB10">
+        <v>15.5075</v>
+      </c>
+      <c r="AC10">
+        <v>15.5075</v>
+      </c>
+      <c r="AD10">
         <v>15.077</v>
       </c>
-      <c r="AA10">
+      <c r="AE10">
         <v>14.47916666666667</v>
       </c>
-      <c r="AB10">
+      <c r="AF10">
         <v>16.874500000000001</v>
       </c>
-      <c r="AC10">
+      <c r="AG10">
+        <v>16.874500000000001</v>
+      </c>
+      <c r="AH10">
         <v>15.099</v>
       </c>
-      <c r="AD10">
+      <c r="AI10">
         <v>16.62</v>
       </c>
-      <c r="AE10">
+      <c r="AJ10">
         <v>17.030999999999999</v>
       </c>
-      <c r="AF10">
+      <c r="AK10">
         <v>19.11</v>
       </c>
-      <c r="AG10">
+      <c r="AL10">
         <v>11.89</v>
       </c>
-      <c r="AH10">
+      <c r="AM10">
         <v>14.62975</v>
       </c>
-      <c r="AI10">
+      <c r="AN10">
         <v>14.465</v>
       </c>
-      <c r="AJ10">
+      <c r="AO10">
+        <v>14.465</v>
+      </c>
+      <c r="AP10">
+        <v>14.465</v>
+      </c>
+      <c r="AQ10">
+        <v>14.465</v>
+      </c>
+      <c r="AR10">
         <v>14.794499999999999</v>
       </c>
-      <c r="AK10">
+      <c r="AS10">
         <v>14.71766666666667</v>
       </c>
-      <c r="AL10">
+      <c r="AT10">
         <v>16.878250000000001</v>
-      </c>
-      <c r="AM10">
-        <v>16.572333333333329</v>
-      </c>
-      <c r="AN10">
-        <v>14.149875</v>
-      </c>
-      <c r="AO10">
-        <v>14.327</v>
-      </c>
-      <c r="AP10">
-        <v>16.572333333333329</v>
-      </c>
-      <c r="AQ10">
-        <v>16.572333333333329</v>
-      </c>
-      <c r="AR10">
-        <v>14.327</v>
-      </c>
-      <c r="AS10">
-        <v>16.572333333333329</v>
-      </c>
-      <c r="AT10">
-        <v>14.327</v>
       </c>
       <c r="AU10">
         <v>16.572333333333329</v>
       </c>
       <c r="AV10">
-        <v>16.572333333333329</v>
+        <v>14.149875</v>
       </c>
       <c r="AW10">
-        <v>16.572333333333329</v>
+        <v>14.327</v>
       </c>
       <c r="AX10">
         <v>16.572333333333329</v>
       </c>
       <c r="AY10">
-        <v>16.022916666666671</v>
+        <v>16.572333333333329</v>
       </c>
       <c r="AZ10">
-        <v>16.572333333333329</v>
+        <v>14.327</v>
       </c>
       <c r="BA10">
         <v>16.572333333333329</v>
       </c>
       <c r="BB10">
+        <v>14.327</v>
+      </c>
+      <c r="BC10">
         <v>16.572333333333329</v>
       </c>
+      <c r="BD10">
+        <v>16.572333333333329</v>
+      </c>
+      <c r="BE10">
+        <v>16.572333333333329</v>
+      </c>
+      <c r="BF10">
+        <v>16.572333333333329</v>
+      </c>
+      <c r="BG10">
+        <v>16.022916666666671</v>
+      </c>
+      <c r="BH10">
+        <v>16.572333333333329</v>
+      </c>
+      <c r="BI10">
+        <v>16.572333333333329</v>
+      </c>
+      <c r="BJ10">
+        <v>16.572333333333329</v>
+      </c>
     </row>
-    <row r="11" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A11">
+        <v>15.308666666666671</v>
+      </c>
+      <c r="B11">
+        <v>14.5715</v>
+      </c>
+      <c r="C11">
         <v>14.648999999999999</v>
       </c>
-      <c r="B11">
+      <c r="D11">
         <v>14.968125000000001</v>
       </c>
-      <c r="C11">
+      <c r="E11">
         <v>14.51466666666667</v>
       </c>
-      <c r="D11">
+      <c r="F11">
         <v>15.802555555555561</v>
       </c>
-      <c r="E11">
+      <c r="G11">
         <v>15.433</v>
       </c>
-      <c r="F11">
+      <c r="H11">
         <v>14.878666666666669</v>
       </c>
-      <c r="G11">
+      <c r="I11">
         <v>15.743722222222219</v>
       </c>
-      <c r="H11">
+      <c r="J11">
         <v>14.88466666666667</v>
       </c>
-      <c r="I11">
+      <c r="K11">
         <v>16.002333333333329</v>
       </c>
-      <c r="J11">
+      <c r="L11">
         <v>14.7605</v>
       </c>
-      <c r="K11">
+      <c r="M11">
         <v>15.5055</v>
-      </c>
-      <c r="L11">
-        <v>14.88466666666667</v>
-      </c>
-      <c r="M11">
-        <v>16.203166666666672</v>
       </c>
       <c r="N11">
         <v>14.88466666666667</v>
       </c>
       <c r="O11">
-        <v>14.88466666666667</v>
+        <v>16.203166666666672</v>
       </c>
       <c r="P11">
         <v>14.88466666666667</v>
       </c>
       <c r="Q11">
+        <v>14.88466666666667</v>
+      </c>
+      <c r="R11">
+        <v>14.88466666666667</v>
+      </c>
+      <c r="S11">
         <v>16.89233333333333</v>
-      </c>
-      <c r="R11">
-        <v>15.28033333333333</v>
-      </c>
-      <c r="S11">
-        <v>16.155000000000001</v>
       </c>
       <c r="T11">
         <v>15.28033333333333</v>
       </c>
       <c r="U11">
-        <v>15.28033333333333</v>
+        <v>16.155000000000001</v>
       </c>
       <c r="V11">
         <v>15.28033333333333</v>
@@ -9963,156 +10249,180 @@
         <v>15.28033333333333</v>
       </c>
       <c r="Z11">
+        <v>15.28033333333333</v>
+      </c>
+      <c r="AA11">
+        <v>15.28033333333333</v>
+      </c>
+      <c r="AB11">
+        <v>15.28033333333333</v>
+      </c>
+      <c r="AC11">
+        <v>15.28033333333333</v>
+      </c>
+      <c r="AD11">
         <v>15.845000000000001</v>
       </c>
-      <c r="AA11">
+      <c r="AE11">
         <v>14.99163636363636</v>
       </c>
-      <c r="AB11">
+      <c r="AF11">
         <v>16.848333333333329</v>
       </c>
-      <c r="AC11">
+      <c r="AG11">
+        <v>16.848333333333329</v>
+      </c>
+      <c r="AH11">
         <v>16.934999999999999</v>
       </c>
-      <c r="AD11">
+      <c r="AI11">
         <v>17.12</v>
       </c>
-      <c r="AE11">
+      <c r="AJ11">
         <v>17.104333333333329</v>
       </c>
-      <c r="AF11">
+      <c r="AK11">
         <v>18.899999999999999</v>
       </c>
-      <c r="AG11">
+      <c r="AL11">
         <v>16.438500000000001</v>
       </c>
-      <c r="AH11">
+      <c r="AM11">
         <v>14.90436666666667</v>
       </c>
-      <c r="AI11">
+      <c r="AN11">
         <v>14.720333333333331</v>
       </c>
-      <c r="AJ11">
+      <c r="AO11">
+        <v>14.720333333333331</v>
+      </c>
+      <c r="AP11">
+        <v>14.720333333333331</v>
+      </c>
+      <c r="AQ11">
+        <v>14.720333333333331</v>
+      </c>
+      <c r="AR11">
         <v>15.0884</v>
       </c>
-      <c r="AK11">
+      <c r="AS11">
         <v>15.590999999999999</v>
       </c>
-      <c r="AL11">
+      <c r="AT11">
         <v>16.118749999999999</v>
-      </c>
-      <c r="AM11">
-        <v>16.155000000000001</v>
-      </c>
-      <c r="AN11">
-        <v>15.39066666666667</v>
-      </c>
-      <c r="AO11">
-        <v>14.88466666666667</v>
-      </c>
-      <c r="AP11">
-        <v>16.155000000000001</v>
-      </c>
-      <c r="AQ11">
-        <v>16.155000000000001</v>
-      </c>
-      <c r="AR11">
-        <v>14.88466666666667</v>
-      </c>
-      <c r="AS11">
-        <v>16.155000000000001</v>
-      </c>
-      <c r="AT11">
-        <v>14.88466666666667</v>
       </c>
       <c r="AU11">
         <v>16.155000000000001</v>
       </c>
       <c r="AV11">
-        <v>16.155000000000001</v>
+        <v>15.39066666666667</v>
       </c>
       <c r="AW11">
-        <v>16.155000000000001</v>
+        <v>14.88466666666667</v>
       </c>
       <c r="AX11">
         <v>16.155000000000001</v>
       </c>
       <c r="AY11">
-        <v>16.07866666666667</v>
+        <v>16.155000000000001</v>
       </c>
       <c r="AZ11">
-        <v>16.155000000000001</v>
+        <v>14.88466666666667</v>
       </c>
       <c r="BA11">
         <v>16.155000000000001</v>
       </c>
       <c r="BB11">
+        <v>14.88466666666667</v>
+      </c>
+      <c r="BC11">
         <v>16.155000000000001</v>
       </c>
+      <c r="BD11">
+        <v>16.155000000000001</v>
+      </c>
+      <c r="BE11">
+        <v>16.155000000000001</v>
+      </c>
+      <c r="BF11">
+        <v>16.155000000000001</v>
+      </c>
+      <c r="BG11">
+        <v>16.07866666666667</v>
+      </c>
+      <c r="BH11">
+        <v>16.155000000000001</v>
+      </c>
+      <c r="BI11">
+        <v>16.155000000000001</v>
+      </c>
+      <c r="BJ11">
+        <v>16.155000000000001</v>
+      </c>
     </row>
-    <row r="12" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A12">
+        <v>14.278</v>
+      </c>
+      <c r="B12">
+        <v>14.241199999999999</v>
+      </c>
+      <c r="C12">
         <v>14.38</v>
       </c>
-      <c r="B12">
+      <c r="D12">
         <v>14.32157142857143</v>
       </c>
-      <c r="C12">
+      <c r="E12">
         <v>14.523418604651161</v>
       </c>
-      <c r="D12">
+      <c r="F12">
         <v>15.670235294117649</v>
       </c>
-      <c r="E12">
+      <c r="G12">
         <v>15.045</v>
       </c>
-      <c r="F12">
+      <c r="H12">
         <v>14.882199999999999</v>
       </c>
-      <c r="G12">
+      <c r="I12">
         <v>18.75075</v>
       </c>
-      <c r="H12">
+      <c r="J12">
         <v>17.189250000000001</v>
       </c>
-      <c r="I12">
+      <c r="K12">
         <v>17.139624999999999</v>
       </c>
-      <c r="J12">
+      <c r="L12">
         <v>14.827999999999999</v>
       </c>
-      <c r="K12">
+      <c r="M12">
         <v>15.3485</v>
-      </c>
-      <c r="L12">
-        <v>17.189250000000001</v>
-      </c>
-      <c r="M12">
-        <v>18.718299999999999</v>
       </c>
       <c r="N12">
         <v>17.189250000000001</v>
       </c>
       <c r="O12">
-        <v>17.189250000000001</v>
+        <v>18.718299999999999</v>
       </c>
       <c r="P12">
         <v>17.189250000000001</v>
       </c>
       <c r="Q12">
+        <v>17.189250000000001</v>
+      </c>
+      <c r="R12">
+        <v>17.189250000000001</v>
+      </c>
+      <c r="S12">
         <v>18.669625</v>
-      </c>
-      <c r="R12">
-        <v>15.00566666666667</v>
-      </c>
-      <c r="S12">
-        <v>18.737500000000001</v>
       </c>
       <c r="T12">
         <v>15.00566666666667</v>
       </c>
       <c r="U12">
-        <v>15.00566666666667</v>
+        <v>18.737500000000001</v>
       </c>
       <c r="V12">
         <v>15.00566666666667</v>
@@ -10127,156 +10437,180 @@
         <v>15.00566666666667</v>
       </c>
       <c r="Z12">
+        <v>15.00566666666667</v>
+      </c>
+      <c r="AA12">
+        <v>15.00566666666667</v>
+      </c>
+      <c r="AB12">
+        <v>15.00566666666667</v>
+      </c>
+      <c r="AC12">
+        <v>15.00566666666667</v>
+      </c>
+      <c r="AD12">
         <v>15.3675</v>
       </c>
-      <c r="AA12">
+      <c r="AE12">
         <v>14.49228571428571</v>
       </c>
-      <c r="AB12">
+      <c r="AF12">
         <v>17.967500000000001</v>
       </c>
-      <c r="AC12">
+      <c r="AG12">
+        <v>17.967500000000001</v>
+      </c>
+      <c r="AH12">
         <v>16.731000000000002</v>
       </c>
-      <c r="AD12">
+      <c r="AI12">
         <v>17.09</v>
       </c>
-      <c r="AE12">
+      <c r="AJ12">
         <v>17.213999999999999</v>
       </c>
-      <c r="AF12">
+      <c r="AK12">
         <v>20.149999999999999</v>
       </c>
-      <c r="AG12">
+      <c r="AL12">
         <v>12.946</v>
       </c>
-      <c r="AH12">
+      <c r="AM12">
         <v>14.814500000000001</v>
       </c>
-      <c r="AI12">
+      <c r="AN12">
         <v>14.41475</v>
       </c>
-      <c r="AJ12">
+      <c r="AO12">
+        <v>14.41475</v>
+      </c>
+      <c r="AP12">
+        <v>14.41475</v>
+      </c>
+      <c r="AQ12">
+        <v>14.41475</v>
+      </c>
+      <c r="AR12">
         <v>15.21425</v>
       </c>
-      <c r="AK12">
+      <c r="AS12">
         <v>14.278</v>
       </c>
-      <c r="AL12">
+      <c r="AT12">
         <v>20.449000000000002</v>
-      </c>
-      <c r="AM12">
-        <v>18.737500000000001</v>
-      </c>
-      <c r="AN12">
-        <v>15.10788888888889</v>
-      </c>
-      <c r="AO12">
-        <v>17.189250000000001</v>
-      </c>
-      <c r="AP12">
-        <v>18.737500000000001</v>
-      </c>
-      <c r="AQ12">
-        <v>18.737500000000001</v>
-      </c>
-      <c r="AR12">
-        <v>17.189250000000001</v>
-      </c>
-      <c r="AS12">
-        <v>18.737500000000001</v>
-      </c>
-      <c r="AT12">
-        <v>17.189250000000001</v>
       </c>
       <c r="AU12">
         <v>18.737500000000001</v>
       </c>
       <c r="AV12">
-        <v>18.737500000000001</v>
+        <v>15.10788888888889</v>
       </c>
       <c r="AW12">
-        <v>18.737500000000001</v>
+        <v>17.189250000000001</v>
       </c>
       <c r="AX12">
         <v>18.737500000000001</v>
       </c>
       <c r="AY12">
-        <v>17.9385625</v>
+        <v>18.737500000000001</v>
       </c>
       <c r="AZ12">
-        <v>18.737500000000001</v>
+        <v>17.189250000000001</v>
       </c>
       <c r="BA12">
         <v>18.737500000000001</v>
       </c>
       <c r="BB12">
+        <v>17.189250000000001</v>
+      </c>
+      <c r="BC12">
         <v>18.737500000000001</v>
       </c>
+      <c r="BD12">
+        <v>18.737500000000001</v>
+      </c>
+      <c r="BE12">
+        <v>18.737500000000001</v>
+      </c>
+      <c r="BF12">
+        <v>18.737500000000001</v>
+      </c>
+      <c r="BG12">
+        <v>17.9385625</v>
+      </c>
+      <c r="BH12">
+        <v>18.737500000000001</v>
+      </c>
+      <c r="BI12">
+        <v>18.737500000000001</v>
+      </c>
+      <c r="BJ12">
+        <v>18.737500000000001</v>
+      </c>
     </row>
-    <row r="13" spans="1:54" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:63" x14ac:dyDescent="0.35">
       <c r="A13">
+        <v>14.59333333333333</v>
+      </c>
+      <c r="B13">
+        <v>14.461833333333329</v>
+      </c>
+      <c r="C13">
         <v>15.061999999999999</v>
       </c>
-      <c r="B13">
+      <c r="D13">
         <v>14.68188888888889</v>
       </c>
-      <c r="C13">
+      <c r="E13">
         <v>14.3776976744186</v>
       </c>
-      <c r="D13">
+      <c r="F13">
         <v>14.863555555555561</v>
       </c>
-      <c r="E13">
+      <c r="G13">
         <v>15.364000000000001</v>
       </c>
-      <c r="F13">
+      <c r="H13">
         <v>14.89423076923077</v>
       </c>
-      <c r="G13">
+      <c r="I13">
         <v>16.855722222222219</v>
       </c>
-      <c r="H13">
+      <c r="J13">
         <v>17.34566666666667</v>
       </c>
-      <c r="I13">
+      <c r="K13">
         <v>17.59783333333333</v>
       </c>
-      <c r="J13">
+      <c r="L13">
         <v>15.132</v>
       </c>
-      <c r="K13">
+      <c r="M13">
         <v>15.929</v>
-      </c>
-      <c r="L13">
-        <v>17.34566666666667</v>
-      </c>
-      <c r="M13">
-        <v>17.64456666666667</v>
       </c>
       <c r="N13">
         <v>17.34566666666667</v>
       </c>
       <c r="O13">
-        <v>17.34566666666667</v>
+        <v>17.64456666666667</v>
       </c>
       <c r="P13">
         <v>17.34566666666667</v>
       </c>
       <c r="Q13">
+        <v>17.34566666666667</v>
+      </c>
+      <c r="R13">
+        <v>17.34566666666667</v>
+      </c>
+      <c r="S13">
         <v>18.827833333333331</v>
-      </c>
-      <c r="R13">
-        <v>15.929</v>
-      </c>
-      <c r="S13">
-        <v>17.381</v>
       </c>
       <c r="T13">
         <v>15.929</v>
       </c>
       <c r="U13">
-        <v>15.929</v>
+        <v>17.381</v>
       </c>
       <c r="V13">
         <v>15.929</v>
@@ -10291,95 +10625,120 @@
         <v>15.929</v>
       </c>
       <c r="Z13">
+        <v>15.929</v>
+      </c>
+      <c r="AA13">
+        <v>15.929</v>
+      </c>
+      <c r="AB13">
+        <v>15.929</v>
+      </c>
+      <c r="AC13">
+        <v>15.929</v>
+      </c>
+      <c r="AD13">
         <v>15.673</v>
       </c>
-      <c r="AA13">
+      <c r="AE13">
         <v>14.9261</v>
       </c>
-      <c r="AB13">
+      <c r="AF13">
         <v>17.623000000000001</v>
       </c>
-      <c r="AC13">
+      <c r="AG13">
+        <v>17.623000000000001</v>
+      </c>
+      <c r="AH13">
         <v>15.996</v>
       </c>
-      <c r="AD13">
+      <c r="AI13">
         <v>17.850000000000001</v>
       </c>
-      <c r="AE13">
+      <c r="AJ13">
         <v>17.451666666666672</v>
       </c>
-      <c r="AF13">
+      <c r="AK13">
         <v>20.309999999999999</v>
       </c>
-      <c r="AG13">
+      <c r="AL13">
         <v>16.920999999999999</v>
       </c>
-      <c r="AH13">
+      <c r="AM13">
         <v>15.159166666666669</v>
       </c>
-      <c r="AI13">
+      <c r="AN13">
         <v>14.846</v>
       </c>
-      <c r="AJ13">
+      <c r="AO13">
+        <v>14.846</v>
+      </c>
+      <c r="AP13">
+        <v>14.846</v>
+      </c>
+      <c r="AQ13">
+        <v>14.846</v>
+      </c>
+      <c r="AR13">
         <v>15.47233333333333</v>
       </c>
-      <c r="AK13">
+      <c r="AS13">
         <v>14.59333333333333</v>
       </c>
-      <c r="AL13">
+      <c r="AT13">
         <v>17.212599999999998</v>
-      </c>
-      <c r="AM13">
-        <v>17.381</v>
-      </c>
-      <c r="AN13">
-        <v>14.93166666666667</v>
-      </c>
-      <c r="AO13">
-        <v>17.34566666666667</v>
-      </c>
-      <c r="AP13">
-        <v>17.381</v>
-      </c>
-      <c r="AQ13">
-        <v>17.381</v>
-      </c>
-      <c r="AR13">
-        <v>17.34566666666667</v>
-      </c>
-      <c r="AS13">
-        <v>17.381</v>
-      </c>
-      <c r="AT13">
-        <v>17.34566666666667</v>
       </c>
       <c r="AU13">
         <v>17.381</v>
       </c>
       <c r="AV13">
-        <v>17.381</v>
+        <v>14.93166666666667</v>
       </c>
       <c r="AW13">
-        <v>17.381</v>
+        <v>17.34566666666667</v>
       </c>
       <c r="AX13">
         <v>17.381</v>
       </c>
       <c r="AY13">
-        <v>17.489416666666671</v>
+        <v>17.381</v>
       </c>
       <c r="AZ13">
-        <v>17.381</v>
+        <v>17.34566666666667</v>
       </c>
       <c r="BA13">
         <v>17.381</v>
       </c>
       <c r="BB13">
+        <v>17.34566666666667</v>
+      </c>
+      <c r="BC13">
+        <v>17.381</v>
+      </c>
+      <c r="BD13">
+        <v>17.381</v>
+      </c>
+      <c r="BE13">
+        <v>17.381</v>
+      </c>
+      <c r="BF13">
+        <v>17.381</v>
+      </c>
+      <c r="BG13">
+        <v>17.489416666666671</v>
+      </c>
+      <c r="BH13">
+        <v>17.381</v>
+      </c>
+      <c r="BI13">
+        <v>17.381</v>
+      </c>
+      <c r="BJ13">
         <v>17.381</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -10387,7 +10746,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>

</xml_diff>